<commit_message>
trace generator and fix bug
</commit_message>
<xml_diff>
--- a/documents/example/windmill-state-d.xlsx
+++ b/documents/example/windmill-state-d.xlsx
@@ -811,9 +811,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AO27" sqref="AO27"/>
+      <selection pane="topRight" activeCell="AO8" sqref="AO8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -823,6 +823,7 @@
     <col min="12" max="12" width="11.25" customWidth="1"/>
     <col min="37" max="37" width="10.125" customWidth="1"/>
     <col min="39" max="39" width="11.25" customWidth="1"/>
+    <col min="45" max="45" width="10.25" customWidth="1"/>
     <col min="47" max="47" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>